<commit_message>
Before moving to get transactional data state
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/alexandra_veizu_uipath_com/Documents/Documents/Projects/FrameworkTemplates/REFramework/VB/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Work Area\UiPath\GenerateOfferLetters\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F8C54E24-BA5C-4BF9-8DAB-2778512EC11B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14A7F095-7132-4215-B69C-343A45469A3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10248" yWindow="17508" windowWidth="21252" windowHeight="9444" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -159,7 +159,7 @@
     <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
   </si>
   <si>
-    <t>ProcessABCQueue</t>
+    <t>HiredCandidates</t>
   </si>
 </sst>
 </file>
@@ -538,15 +538,15 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5546875" customWidth="1"/>
+    <col min="1" max="1" width="43.5703125" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="81.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -594,7 +594,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:26" ht="45">
       <c r="A3" s="2" t="s">
         <v>31</v>
       </c>
@@ -604,7 +604,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="28.8">
+    <row r="5" spans="1:26" ht="30">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -1623,12 +1623,12 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="75.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1665,7 +1665,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="28.8">
+    <row r="2" spans="1:26" ht="30">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1676,7 +1676,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:26" ht="45">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -1790,7 +1790,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="28.8">
+    <row r="17" spans="1:3" ht="45">
       <c r="A17" t="s">
         <v>40</v>
       </c>
@@ -2786,12 +2786,12 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.88671875" customWidth="1"/>
-    <col min="2" max="2" width="30.109375" customWidth="1"/>
-    <col min="3" max="3" width="60.33203125" customWidth="1"/>
-    <col min="4" max="26" width="65.44140625" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" customWidth="1"/>
+    <col min="3" max="3" width="60.28515625" customWidth="1"/>
+    <col min="4" max="26" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>